<commit_message>
Configuración de la segunda pestaña del excel
</commit_message>
<xml_diff>
--- a/downloads/12345678908/jdelgadob-compromiso-plantilla.xlsx
+++ b/downloads/12345678908/jdelgadob-compromiso-plantilla.xlsx
@@ -5,6 +5,7 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Compromisos" r:id="rId4"/>
+    <sheet sheetId="2" name="Leyenda" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="nrocorrelativo">Compromisos!$A$1:$A$2</definedName>
@@ -112,21 +113,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,8 +468,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="16" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -539,6 +544,26 @@
         <v>16</v>
       </c>
     </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:P1"/>
@@ -546,4 +571,14 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cambio de letra a comfortaa y cambio de dirección de correo para envio de notificaciones por email
</commit_message>
<xml_diff>
--- a/downloads/12345678908/jdelgadob-compromiso-plantilla.xlsx
+++ b/downloads/12345678908/jdelgadob-compromiso-plantilla.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
   <si>
     <t>Matriz Integrada de Compromisos de la Unidad de Multiunidad</t>
   </si>
@@ -81,6 +81,153 @@
   </si>
   <si>
     <t>Post-cierre</t>
+  </si>
+  <si>
+    <t>Descripción de los campos.</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Número del compromiso para la tabla. Inicia en 1 y es correlativo.</t>
+  </si>
+  <si>
+    <t>Origen compromiso</t>
+  </si>
+  <si>
+    <t>Estudio origen del compromiso.</t>
+  </si>
+  <si>
+    <t>Capítulo del origen del compromiso.</t>
+  </si>
+  <si>
+    <t>Sección del origen del compromiso.</t>
+  </si>
+  <si>
+    <t>Página del origen del compromiso.</t>
+  </si>
+  <si>
+    <t>Aspecto asociado</t>
+  </si>
+  <si>
+    <t>El aspecto ambiental sobre el cual el compromiso busca gestionar (prevenir, mitigar, compensar, etc) el impacto.</t>
+  </si>
+  <si>
+    <t>Instalación/componente</t>
+  </si>
+  <si>
+    <t>Instalación o componente a la cual el compromiso se encuentra vinculada.</t>
+  </si>
+  <si>
+    <t>Es el copia textual del compromiso tal y como se presentó en el estudio origen.</t>
+  </si>
+  <si>
+    <t>Resumen del compromiso</t>
+  </si>
+  <si>
+    <t>Es un texto que presenta de manera resumida el compromiso.</t>
+  </si>
+  <si>
+    <t>Antecedentes del compromiso</t>
+  </si>
+  <si>
+    <t>Es un texto que presenta información sobre los antecedentes del compromiso como por ejemplo si es que representa una actualiza, abarca o reemplaza un compromiso anterior, similar o duplicado.</t>
+  </si>
+  <si>
+    <t>Establece si el compromiso ocurre una vez de manera puntual o de manera permanente dentro del periodo de vigencia.</t>
+  </si>
+  <si>
+    <t>Fecha en la que se iniciará el compromiso.</t>
+  </si>
+  <si>
+    <t>Establece la frecuencia de cumplimiento del compromiso dentro del periodo de vigencia.</t>
+  </si>
+  <si>
+    <t>Calificación cualitativa sobre la criticidad del compromiso a distintas características como el riesgo, las consecuencias, etc.</t>
+  </si>
+  <si>
+    <t>Evidencias</t>
+  </si>
+  <si>
+    <t>Indica la existencia de evidencia de cumplimiento e incluye los archivos correspondientes.</t>
+  </si>
+  <si>
+    <t>Señala la situación de cumplimiento del compromiso.</t>
+  </si>
+  <si>
+    <t>Acción sobre el compromiso</t>
+  </si>
+  <si>
+    <t>Señala si se requiere alguna acción sobre el compromiso.</t>
+  </si>
+  <si>
+    <t>Detalle de acción</t>
+  </si>
+  <si>
+    <t>Detalle de la acción que requiere.</t>
+  </si>
+  <si>
+    <t>Frecuencia de verificación</t>
+  </si>
+  <si>
+    <t>Cada cuanto tiempo se verificará el cumplimiento de un compromiso.</t>
+  </si>
+  <si>
+    <t>Area responsable</t>
+  </si>
+  <si>
+    <t>Señala el equipo o área responsable de ejecutar el compromiso.</t>
+  </si>
+  <si>
+    <t>Correos de notificación</t>
+  </si>
+  <si>
+    <t>Lista de correos para notificaciones y avisos de verificación.</t>
+  </si>
+  <si>
+    <t>Notificación de inactividad</t>
+  </si>
+  <si>
+    <t>No Definido</t>
+  </si>
+  <si>
+    <t>Nombre de revisor</t>
+  </si>
+  <si>
+    <t>Nombre del encargado de la revisión.</t>
+  </si>
+  <si>
+    <t>Indica la última vez que el compromiso y sus características fueron revisadas y validadas.</t>
+  </si>
+  <si>
+    <t>Referencia técnica o legal de cumplimiento</t>
+  </si>
+  <si>
+    <t>Indica, en caso exista, la referencia sobre cómo se deberá cumplir el compromiso en base a la normativa o texto técnico.</t>
+  </si>
+  <si>
+    <t>Presupuesto</t>
+  </si>
+  <si>
+    <t>Indica el presupuesto asociado al cumplimiento.</t>
+  </si>
+  <si>
+    <t>Permite complementar el compromiso con detalles específicos.</t>
+  </si>
+  <si>
+    <t>Establece el periodo de construcción y si es que el compromiso está vigente en  esta etapa.</t>
+  </si>
+  <si>
+    <t>Establece el periodo de operación y si es que el compromiso está vigente en  esta etapa.</t>
+  </si>
+  <si>
+    <t>Establece el periodo de cierre y si es que el compromiso está vigente en  esta etapa.</t>
+  </si>
+  <si>
+    <t>Establece el periodo de post-cierre y si es que el compromiso está vigente en  esta etapa.</t>
   </si>
 </sst>
 </file>
@@ -575,9 +722,275 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B33"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="180" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>